<commit_message>
changed cheat sheet to add Scotty's && ||
</commit_message>
<xml_diff>
--- a/javascript cheat sheet.xlsx
+++ b/javascript cheat sheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="23320" yWindow="-120" windowWidth="22580" windowHeight="26020" tabRatio="500"/>
+    <workbookView xWindow="160" yWindow="-60" windowWidth="21600" windowHeight="13900" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,643 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="207">
+  <si>
+    <t>array can store arrays - multi-dimensional array</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>var cars = [toyotas, porsches];</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>var toyotas = ["A", "B"];</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>var porsches = ["C", "D"];</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. declare variable</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2. assign value</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>OR - both at once</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>var name = "Jeff";</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>console.log(name);</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&gt;Jeff</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>no need to redeclare</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>name = "Steve";</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&gt;Steve</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>once declared, can change value</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>comment out</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>command-/</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>multi</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>log in to console</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>console log</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>alert</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>always end with</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>basic math</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>10 + 10;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&gt;20</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>var x = 100;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&gt;4000</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>x * 40;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>string concatenation - connect strings</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&gt;HelloClass</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;script src = "main.js"&gt;&lt;/script&gt;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>//</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>console.log("Hello");</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>alert("Hello");</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>string - text itself</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>"Hello"</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>5, 5.5, 1000</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>number - all are floats</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>boolean</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>true, false</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>undefined</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>no value</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>var name;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>var name = "Jeff";</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&gt;false</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&amp;&amp;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>||</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>!</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>not</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>!= - value</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>!== - value and type</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>and - true if both true, otherwise false</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>or - true if either one true, if both are false then false</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>not equal</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>also</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;, &gt;, &lt;=, &gt;=</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>5&gt;10;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>if (5&gt;10) {</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">  console.log("won't see");</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>if (5&lt;10) {</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">  console.log("will see");</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>else - runs only if "if" evaluates to false</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>if (5&gt;10) {</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>} else {</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>var x = 2</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>if (x&lt;10) {</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">  alert(x + " is less than 10");</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">  console.log("Your var was " + x + " and is not less than 10");</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>else if</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>} else if (5 === 5) {</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">  console.log("won't get here");</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>or - var cars =  ["A", "B"], ["C", "D"];</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>console.log(cars[1][0]);</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&gt;C</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. create object with strings for keys</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>var car = {make: 'Toyota', model: 'Prius'};</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2. retrieve data with bracket notation</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>console.log(car['make']);</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>or - "dot notation" to retrieve data</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>var user = {first: 'John', last: 'Smith'};</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>console.log(user.first);</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&gt;"John"</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&gt;"Toyota"</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>/* multi</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>line "block"</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>comment */</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>can put over multiple lines</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>var user = {</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">  first: "John",</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">  last: "Smith"</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>};</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>value comparison</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>"hi" = "hi"     &gt;true</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>"hi" = bye"    &gt;false</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>"Hello" + "Class";</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>[11, "elephant"];</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>can be stored as variable</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>var class_names = ["Julie", "Rob"];</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>access - index of item is numbered position,</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>starting at zero</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>myArray[0]</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. declare array</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2. access element</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>["Snoopy", "Charlie", "Patty"];</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>peanuts = ["Snoopy", "Charlie", "Patty"];</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>console.log(peanuts[0]);</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;Snoopy</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>i=0</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1&lt;10</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>define - value before iteration,</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>a condition under which the loops continues,</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>how it changes value after each iteration</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>i++1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">  console.log(SnoopyPosition);</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">  var SnoopyPosition = peanuts.indexOf("Snoopy");</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&gt;0 … 9</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&gt;3</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>a function can return only once then ends,</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>can't add another variable and return after first</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>function getName(name) {</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">  console.log("Hi " + name);</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>getName("Irin");</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&gt;Hi Irin</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">  return sum;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>var mySum = addNums(1,2);</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>function shoo() {</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">  console.log("Go away!");</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&gt;Go away!</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>no arguments</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>shoo();</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>check data type of assigned value, type of operator</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>var yourData = "Data";</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&gt;String</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>index of - to check index of a particular value</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>var peanuts = ["Charlie", "Snoopy"];</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">  console.log(typeOf yourData);</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&gt;1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>to encapsulate code for later use</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. define - what want function to do</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2. call - tell function to execute</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>function shoutHello() {</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">  alert("Hello");</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>shoutHello();</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>accessed outside of function definition</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. definte</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>function shoutToWorld(myString) {</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">  alert(myString);</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">  console.log(myString);</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2. call</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>shoutToWorld("Hi");</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>but can't access myString here</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>return - to access value outside function</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>function addNums(num1, num2) {</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">  var sum = num1 + num2;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>call</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>(10 - 5) == "5"    &gt;true - only checks value, not type</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>(10 - 5) == 5       &gt;true</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>(10 - 5) === "5"  &gt;false - checks value and type</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
   <si>
     <t>command-option-j, &gt;&gt; to console</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -300,614 +936,6 @@
   </si>
   <si>
     <t>times using iterator variable</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>i=0</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>1&lt;10</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>define - value before iteration,</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>a condition under which the loops continues,</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>how it changes value after each iteration</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>i++1</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">  console.log(SnoopyPosition);</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">  var SnoopyPosition = peanuts.indexOf("Snoopy");</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>&gt;0 … 9</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>&gt;3</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>a function can return only once then ends,</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>can't add another variable and return after first</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>function getName(name) {</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">  console.log("Hi " + name);</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>getName("Irin");</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>&gt;Hi Irin</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">  return sum;</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>var mySum = addNums(1,2);</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>function shoo() {</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">  console.log("Go away!");</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>&gt;Go away!</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>no arguments</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>shoo();</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>check data type of assigned value, type of operator</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>var yourData = "Data";</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>&gt;String</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>index of - to check index of a particular value</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>var peanuts = ["Charlie", "Snoopy"];</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">  console.log(typeOf yourData);</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>&gt;1</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>to encapsulate code for later use</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>1. define - what want function to do</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>2. call - tell function to execute</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>function shoutHello() {</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">  alert("Hello");</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>shoutHello();</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>accessed outside of function definition</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>1. definte</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>function shoutToWorld(myString) {</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">  alert(myString);</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">  console.log(myString);</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>2. call</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>shoutToWorld("Hi");</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>but can't access myString here</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>return - to access value outside function</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>function addNums(num1, num2) {</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">  var sum = num1 + num2;</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>call</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>(10 - 5) == "5"    &gt;true - only checks value, not type</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>(10 - 5) == 5       &gt;true</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>(10 - 5) === "5"  &gt;false - checks value and type</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>not equal</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>!==</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>also</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;, &gt;, &lt;=, &gt;=</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>5&gt;10;</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>&gt;false</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>if (5&gt;10) {</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>}</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">  console.log("won't see");</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>if (5&lt;10) {</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">  console.log("will see");</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>else - runs only if "if" evaluates to false</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>if (5&gt;10) {</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>} else {</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>var x = 2</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>if (x&lt;10) {</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">  alert(x + " is less than 10");</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">  console.log("Your var was " + x + " and is not less than 10");</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>else if</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>} else if (5 === 5) {</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">  console.log("won't get here");</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>or - var cars =  ["A", "B"], ["C", "D"];</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>console.log(cars[1][0]);</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>&gt;C</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>1. create object with strings for keys</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>var car = {make: 'Toyota', model: 'Prius'};</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>2. retrieve data with bracket notation</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>console.log(car['make']);</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>or - "dot notation" to retrieve data</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>var user = {first: 'John', last: 'Smith'};</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>console.log(user.first);</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>&gt;"John"</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>&gt;"Toyota"</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>/* multi</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>line "block"</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>comment */</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>can put over multiple lines</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>var user = {</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">  first: "John",</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">  last: "Smith"</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>};</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>value comparison</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>"hi" = "hi"     &gt;true</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>"hi" = bye"    &gt;false</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>"Hello" + "Class";</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>[11, "elephant"];</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>can be stored as variable</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>var class_names = ["Julie", "Rob"];</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>access - index of item is numbered position,</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>starting at zero</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>myArray[0]</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>1. declare array</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>2. access element</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>["Snoopy", "Charlie", "Patty"];</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>peanuts = ["Snoopy", "Charlie", "Patty"];</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>console.log(peanuts[0]);</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;Snoopy</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>array can store arrays - multi-dimensional array</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>var cars = [toyotas, porsches];</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>var toyotas = ["A", "B"];</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>var porsches = ["C", "D"];</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>1. declare variable</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>2. assign value</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>OR - both at once</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>var name = "Jeff";</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>console.log(name);</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>&gt;Jeff</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>no need to redeclare</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>name = "Steve";</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>&gt;Steve</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>once declared, can change value</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>comment out</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>command-/</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>multi</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>log in to console</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>console log</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>alert</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>always end with</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>basic math</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>10 + 10;</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>&gt;20</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>var x = 100;</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>&gt;4000</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>x * 40;</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>string concatenation - connect strings</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>&gt;HelloClass</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;script src = "main.js"&gt;&lt;/script&gt;</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>//</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>console.log("Hello");</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>alert("Hello");</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>string - text itself</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>"Hello"</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>5, 5.5, 1000</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>number - all are floats</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>boolean</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>true, false</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>undefined</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>no value</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>var name;</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>;</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>var name = "Jeff";</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1411,7 +1439,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="18">
       <c r="A1" s="2" t="s">
-        <v>36</v>
+        <v>195</v>
       </c>
       <c r="B1" s="1">
         <v>40824</v>
@@ -1419,10 +1447,10 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="4" t="s">
-        <v>37</v>
+        <v>196</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>185</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1431,336 +1459,336 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="4" t="s">
-        <v>2</v>
+        <v>161</v>
       </c>
       <c r="B6" s="5"/>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="8" t="s">
-        <v>13</v>
+        <v>172</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>186</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="8" t="s">
-        <v>172</v>
+        <v>16</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>132</v>
+        <v>84</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="8"/>
       <c r="B9" s="9" t="s">
-        <v>133</v>
+        <v>85</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="8"/>
       <c r="B10" s="9" t="s">
-        <v>134</v>
+        <v>86</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="10" t="s">
-        <v>170</v>
+        <v>14</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>171</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="6" t="s">
-        <v>173</v>
+        <v>17</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>0</v>
+        <v>159</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="8" t="s">
-        <v>174</v>
+        <v>18</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>187</v>
+        <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="10" t="s">
-        <v>175</v>
+        <v>19</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>188</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="4" t="s">
-        <v>3</v>
+        <v>162</v>
       </c>
       <c r="B16" s="5"/>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="6" t="s">
-        <v>189</v>
+        <v>33</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>190</v>
+        <v>34</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="8" t="s">
-        <v>192</v>
+        <v>36</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>191</v>
+        <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="8" t="s">
-        <v>193</v>
+        <v>37</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>194</v>
+        <v>38</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="10" t="s">
-        <v>195</v>
+        <v>39</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>196</v>
+        <v>40</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="13" t="s">
-        <v>1</v>
+        <v>160</v>
       </c>
       <c r="B22" s="7"/>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="8" t="s">
-        <v>160</v>
+        <v>4</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>197</v>
+        <v>41</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" s="8" t="s">
-        <v>161</v>
+        <v>5</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>199</v>
+        <v>43</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" s="8" t="s">
-        <v>162</v>
+        <v>6</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>163</v>
+        <v>7</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" s="8"/>
       <c r="B26" s="9" t="s">
-        <v>164</v>
+        <v>8</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" s="8"/>
       <c r="B27" s="9" t="s">
-        <v>165</v>
+        <v>9</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" s="8" t="s">
-        <v>169</v>
+        <v>13</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>167</v>
+        <v>11</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" s="8" t="s">
-        <v>166</v>
+        <v>10</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>164</v>
+        <v>8</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" s="10"/>
       <c r="B30" s="11" t="s">
-        <v>168</v>
+        <v>12</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" s="12" t="s">
-        <v>176</v>
+        <v>20</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>198</v>
+        <v>42</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="6" t="s">
-        <v>177</v>
+        <v>21</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>178</v>
+        <v>22</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34" s="8"/>
       <c r="B34" s="9" t="s">
-        <v>179</v>
+        <v>23</v>
       </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35" s="8"/>
       <c r="B35" s="9" t="s">
-        <v>180</v>
+        <v>24</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36" s="8"/>
       <c r="B36" s="9" t="s">
-        <v>182</v>
+        <v>26</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" s="8"/>
       <c r="B37" s="9" t="s">
-        <v>181</v>
+        <v>25</v>
       </c>
     </row>
     <row r="38" spans="1:2">
       <c r="A38" s="8" t="s">
-        <v>42</v>
+        <v>201</v>
       </c>
       <c r="B38" s="9" t="s">
-        <v>44</v>
+        <v>203</v>
       </c>
     </row>
     <row r="39" spans="1:2">
       <c r="A39" s="10" t="s">
-        <v>43</v>
+        <v>202</v>
       </c>
       <c r="B39" s="11" t="s">
-        <v>45</v>
+        <v>204</v>
       </c>
     </row>
     <row r="40" spans="1:2">
       <c r="A40" s="6" t="s">
-        <v>183</v>
+        <v>27</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>143</v>
+        <v>95</v>
       </c>
     </row>
     <row r="41" spans="1:2">
       <c r="A41" s="10"/>
       <c r="B41" s="11" t="s">
-        <v>184</v>
+        <v>28</v>
       </c>
     </row>
     <row r="43" spans="1:2">
       <c r="A43" s="13" t="s">
-        <v>4</v>
+        <v>163</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>152</v>
+        <v>104</v>
       </c>
     </row>
     <row r="44" spans="1:2">
       <c r="A44" s="8"/>
       <c r="B44" s="9" t="s">
-        <v>144</v>
+        <v>96</v>
       </c>
     </row>
     <row r="45" spans="1:2">
       <c r="A45" s="8" t="s">
-        <v>145</v>
+        <v>97</v>
       </c>
       <c r="B45" s="9" t="s">
-        <v>146</v>
+        <v>98</v>
       </c>
     </row>
     <row r="46" spans="1:2">
       <c r="A46" s="8" t="s">
-        <v>147</v>
+        <v>99</v>
       </c>
       <c r="B46" s="9" t="s">
-        <v>149</v>
+        <v>101</v>
       </c>
     </row>
     <row r="47" spans="1:2">
       <c r="A47" s="8" t="s">
-        <v>148</v>
+        <v>100</v>
       </c>
       <c r="B47" s="9"/>
     </row>
     <row r="48" spans="1:2">
       <c r="A48" s="8" t="s">
-        <v>150</v>
+        <v>102</v>
       </c>
       <c r="B48" s="9" t="s">
-        <v>153</v>
+        <v>105</v>
       </c>
     </row>
     <row r="49" spans="1:2">
       <c r="A49" s="8" t="s">
-        <v>151</v>
+        <v>103</v>
       </c>
       <c r="B49" s="9" t="s">
-        <v>154</v>
+        <v>106</v>
       </c>
     </row>
     <row r="50" spans="1:2">
       <c r="A50" s="8"/>
       <c r="B50" s="9" t="s">
-        <v>155</v>
+        <v>107</v>
       </c>
     </row>
     <row r="51" spans="1:2">
       <c r="A51" s="8" t="s">
-        <v>156</v>
+        <v>0</v>
       </c>
       <c r="B51" s="9" t="s">
-        <v>158</v>
+        <v>2</v>
       </c>
     </row>
     <row r="52" spans="1:2">
       <c r="A52" s="8"/>
       <c r="B52" s="9" t="s">
-        <v>159</v>
+        <v>3</v>
       </c>
     </row>
     <row r="53" spans="1:2">
       <c r="A53" s="8"/>
       <c r="B53" s="9" t="s">
-        <v>157</v>
+        <v>1</v>
       </c>
     </row>
     <row r="54" spans="1:2">
       <c r="A54" s="8"/>
       <c r="B54" s="9" t="s">
-        <v>120</v>
+        <v>72</v>
       </c>
     </row>
     <row r="55" spans="1:2">
       <c r="A55" s="8"/>
       <c r="B55" s="9" t="s">
-        <v>121</v>
+        <v>73</v>
       </c>
     </row>
     <row r="56" spans="1:2">
       <c r="A56" s="10"/>
       <c r="B56" s="11" t="s">
-        <v>122</v>
+        <v>74</v>
       </c>
     </row>
     <row r="57" spans="1:2">
@@ -1777,664 +1805,694 @@
     </row>
     <row r="61" spans="1:2">
       <c r="A61" s="13" t="s">
-        <v>5</v>
+        <v>164</v>
       </c>
       <c r="B61" s="7"/>
     </row>
     <row r="62" spans="1:2">
       <c r="A62" s="8" t="s">
-        <v>123</v>
+        <v>75</v>
       </c>
       <c r="B62" s="9" t="s">
-        <v>124</v>
+        <v>76</v>
       </c>
     </row>
     <row r="63" spans="1:2">
       <c r="A63" s="8" t="s">
-        <v>125</v>
+        <v>77</v>
       </c>
       <c r="B63" s="9" t="s">
-        <v>126</v>
+        <v>78</v>
       </c>
     </row>
     <row r="64" spans="1:2">
       <c r="A64" s="8"/>
       <c r="B64" s="9" t="s">
-        <v>131</v>
+        <v>83</v>
       </c>
     </row>
     <row r="65" spans="1:2">
       <c r="A65" s="8" t="s">
-        <v>127</v>
+        <v>79</v>
       </c>
       <c r="B65" s="9" t="s">
-        <v>128</v>
+        <v>80</v>
       </c>
     </row>
     <row r="66" spans="1:2">
       <c r="A66" s="8"/>
       <c r="B66" s="9" t="s">
-        <v>129</v>
+        <v>81</v>
       </c>
     </row>
     <row r="67" spans="1:2">
       <c r="A67" s="8"/>
       <c r="B67" s="9" t="s">
-        <v>130</v>
+        <v>82</v>
       </c>
     </row>
     <row r="68" spans="1:2">
       <c r="A68" s="8" t="s">
-        <v>135</v>
+        <v>87</v>
       </c>
       <c r="B68" s="9" t="s">
-        <v>136</v>
+        <v>88</v>
       </c>
     </row>
     <row r="69" spans="1:2">
       <c r="A69" s="8"/>
       <c r="B69" s="9" t="s">
-        <v>137</v>
+        <v>89</v>
       </c>
     </row>
     <row r="70" spans="1:2">
       <c r="A70" s="8"/>
       <c r="B70" s="9" t="s">
-        <v>138</v>
+        <v>90</v>
       </c>
     </row>
     <row r="71" spans="1:2">
       <c r="A71" s="10"/>
       <c r="B71" s="11" t="s">
-        <v>139</v>
+        <v>91</v>
       </c>
     </row>
     <row r="73" spans="1:2">
       <c r="A73" s="13" t="s">
-        <v>6</v>
+        <v>165</v>
       </c>
       <c r="B73" s="7"/>
     </row>
     <row r="74" spans="1:2">
       <c r="A74" s="8" t="s">
-        <v>140</v>
+        <v>92</v>
       </c>
       <c r="B74" s="9" t="s">
-        <v>141</v>
+        <v>93</v>
       </c>
     </row>
     <row r="75" spans="1:2">
       <c r="A75" s="8"/>
       <c r="B75" s="9" t="s">
-        <v>142</v>
+        <v>94</v>
       </c>
     </row>
     <row r="76" spans="1:2">
       <c r="A76" s="8"/>
       <c r="B76" s="9" t="s">
-        <v>97</v>
+        <v>157</v>
       </c>
     </row>
     <row r="77" spans="1:2">
       <c r="A77" s="8"/>
       <c r="B77" s="9" t="s">
-        <v>96</v>
+        <v>156</v>
       </c>
     </row>
     <row r="78" spans="1:2">
       <c r="A78" s="8"/>
       <c r="B78" s="9" t="s">
-        <v>98</v>
+        <v>158</v>
       </c>
     </row>
     <row r="79" spans="1:2">
       <c r="A79" s="8" t="s">
-        <v>99</v>
+        <v>53</v>
       </c>
       <c r="B79" s="9" t="s">
-        <v>100</v>
+        <v>49</v>
       </c>
     </row>
     <row r="80" spans="1:2">
-      <c r="A80" s="8" t="s">
-        <v>101</v>
-      </c>
+      <c r="A80" s="8"/>
       <c r="B80" s="9" t="s">
-        <v>102</v>
+        <v>50</v>
       </c>
     </row>
     <row r="81" spans="1:2">
-      <c r="A81" s="8"/>
+      <c r="A81" s="8" t="s">
+        <v>54</v>
+      </c>
       <c r="B81" s="9" t="s">
-        <v>103</v>
+        <v>55</v>
       </c>
     </row>
     <row r="82" spans="1:2">
-      <c r="A82" s="10"/>
-      <c r="B82" s="11" t="s">
-        <v>104</v>
+      <c r="A82" s="8"/>
+      <c r="B82" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2">
+      <c r="A83" s="8"/>
+      <c r="B83" s="9" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="84" spans="1:2">
-      <c r="A84" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="B84" s="7" t="s">
-        <v>105</v>
+      <c r="A84" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B84" s="9" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="85" spans="1:2">
-      <c r="A85" s="8"/>
+      <c r="A85" s="8" t="s">
+        <v>46</v>
+      </c>
       <c r="B85" s="9" t="s">
-        <v>107</v>
+        <v>52</v>
       </c>
     </row>
     <row r="86" spans="1:2">
-      <c r="A86" s="8"/>
-      <c r="B86" s="9" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2">
-      <c r="A87" s="8"/>
-      <c r="B87" s="9" t="s">
-        <v>108</v>
+      <c r="A86" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="B86" s="11" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="88" spans="1:2">
-      <c r="A88" s="8"/>
-      <c r="B88" s="9" t="s">
-        <v>109</v>
+      <c r="A88" s="13" t="s">
+        <v>166</v>
+      </c>
+      <c r="B88" s="7" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="89" spans="1:2">
       <c r="A89" s="8"/>
       <c r="B89" s="9" t="s">
-        <v>106</v>
+        <v>59</v>
       </c>
     </row>
     <row r="90" spans="1:2">
-      <c r="A90" s="8" t="s">
-        <v>110</v>
-      </c>
+      <c r="A90" s="8"/>
       <c r="B90" s="9" t="s">
-        <v>111</v>
+        <v>58</v>
       </c>
     </row>
     <row r="91" spans="1:2">
       <c r="A91" s="8"/>
       <c r="B91" s="9" t="s">
-        <v>107</v>
+        <v>60</v>
       </c>
     </row>
     <row r="92" spans="1:2">
       <c r="A92" s="8"/>
       <c r="B92" s="9" t="s">
-        <v>112</v>
+        <v>61</v>
       </c>
     </row>
     <row r="93" spans="1:2">
       <c r="A93" s="8"/>
       <c r="B93" s="9" t="s">
-        <v>109</v>
+        <v>58</v>
       </c>
     </row>
     <row r="94" spans="1:2">
-      <c r="A94" s="8"/>
+      <c r="A94" s="8" t="s">
+        <v>62</v>
+      </c>
       <c r="B94" s="9" t="s">
-        <v>106</v>
+        <v>63</v>
       </c>
     </row>
     <row r="95" spans="1:2">
       <c r="A95" s="8"/>
-      <c r="B95" s="9"/>
+      <c r="B95" s="9" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="96" spans="1:2">
       <c r="A96" s="8"/>
       <c r="B96" s="9" t="s">
-        <v>113</v>
+        <v>64</v>
       </c>
     </row>
     <row r="97" spans="1:2">
       <c r="A97" s="8"/>
       <c r="B97" s="9" t="s">
-        <v>114</v>
+        <v>61</v>
       </c>
     </row>
     <row r="98" spans="1:2">
       <c r="A98" s="8"/>
       <c r="B98" s="9" t="s">
-        <v>115</v>
+        <v>58</v>
       </c>
     </row>
     <row r="99" spans="1:2">
       <c r="A99" s="8"/>
-      <c r="B99" s="9" t="s">
-        <v>112</v>
-      </c>
+      <c r="B99" s="9"/>
     </row>
     <row r="100" spans="1:2">
       <c r="A100" s="8"/>
       <c r="B100" s="9" t="s">
-        <v>116</v>
+        <v>65</v>
       </c>
     </row>
     <row r="101" spans="1:2">
       <c r="A101" s="8"/>
       <c r="B101" s="9" t="s">
-        <v>106</v>
+        <v>66</v>
       </c>
     </row>
     <row r="102" spans="1:2">
-      <c r="A102" s="8" t="s">
-        <v>117</v>
-      </c>
+      <c r="A102" s="8"/>
       <c r="B102" s="9" t="s">
-        <v>105</v>
+        <v>67</v>
       </c>
     </row>
     <row r="103" spans="1:2">
       <c r="A103" s="8"/>
       <c r="B103" s="9" t="s">
-        <v>107</v>
+        <v>64</v>
       </c>
     </row>
     <row r="104" spans="1:2">
       <c r="A104" s="8"/>
       <c r="B104" s="9" t="s">
-        <v>118</v>
+        <v>68</v>
       </c>
     </row>
     <row r="105" spans="1:2">
       <c r="A105" s="8"/>
       <c r="B105" s="9" t="s">
-        <v>109</v>
+        <v>58</v>
       </c>
     </row>
     <row r="106" spans="1:2">
-      <c r="A106" s="8"/>
+      <c r="A106" s="8" t="s">
+        <v>69</v>
+      </c>
       <c r="B106" s="9" t="s">
-        <v>112</v>
+        <v>57</v>
       </c>
     </row>
     <row r="107" spans="1:2">
       <c r="A107" s="8"/>
       <c r="B107" s="9" t="s">
-        <v>119</v>
+        <v>59</v>
       </c>
     </row>
     <row r="108" spans="1:2">
-      <c r="A108" s="10"/>
-      <c r="B108" s="11" t="s">
-        <v>106</v>
+      <c r="A108" s="8"/>
+      <c r="B108" s="9" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2">
+      <c r="A109" s="8"/>
+      <c r="B109" s="9" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2">
+      <c r="A110" s="8"/>
+      <c r="B110" s="9" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2">
+      <c r="A111" s="8"/>
+      <c r="B111" s="9" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2">
+      <c r="A112" s="10"/>
+      <c r="B112" s="11" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="122" spans="1:2">
       <c r="A122" s="13" t="s">
-        <v>8</v>
+        <v>167</v>
       </c>
       <c r="B122" s="7"/>
     </row>
     <row r="123" spans="1:2">
       <c r="A123" s="8" t="s">
-        <v>78</v>
+        <v>138</v>
       </c>
       <c r="B123" s="9"/>
     </row>
     <row r="124" spans="1:2">
       <c r="A124" s="8" t="s">
-        <v>79</v>
+        <v>139</v>
       </c>
       <c r="B124" s="9" t="s">
-        <v>81</v>
+        <v>141</v>
       </c>
     </row>
     <row r="125" spans="1:2">
       <c r="A125" s="8"/>
       <c r="B125" s="9" t="s">
-        <v>82</v>
+        <v>142</v>
       </c>
     </row>
     <row r="126" spans="1:2">
       <c r="A126" s="8" t="s">
-        <v>80</v>
+        <v>140</v>
       </c>
       <c r="B126" s="9" t="s">
-        <v>83</v>
+        <v>143</v>
       </c>
     </row>
     <row r="127" spans="1:2">
       <c r="A127" s="14" t="s">
-        <v>9</v>
+        <v>168</v>
       </c>
       <c r="B127" s="9"/>
     </row>
     <row r="128" spans="1:2">
       <c r="A128" s="8" t="s">
-        <v>84</v>
+        <v>144</v>
       </c>
       <c r="B128" s="9"/>
     </row>
     <row r="129" spans="1:2">
       <c r="A129" s="8" t="s">
-        <v>85</v>
+        <v>145</v>
       </c>
       <c r="B129" s="9" t="s">
-        <v>86</v>
+        <v>146</v>
       </c>
     </row>
     <row r="130" spans="1:2">
       <c r="A130" s="8"/>
       <c r="B130" s="9" t="s">
-        <v>88</v>
+        <v>148</v>
       </c>
     </row>
     <row r="131" spans="1:2">
       <c r="A131" s="8"/>
       <c r="B131" s="9" t="s">
-        <v>87</v>
+        <v>147</v>
       </c>
     </row>
     <row r="132" spans="1:2">
       <c r="A132" s="8"/>
       <c r="B132" s="9" t="s">
-        <v>106</v>
+        <v>58</v>
       </c>
     </row>
     <row r="133" spans="1:2">
       <c r="A133" s="8" t="s">
-        <v>89</v>
+        <v>149</v>
       </c>
       <c r="B133" s="9" t="s">
-        <v>90</v>
+        <v>150</v>
       </c>
     </row>
     <row r="134" spans="1:2">
       <c r="A134" s="8" t="s">
-        <v>91</v>
+        <v>151</v>
       </c>
       <c r="B134" s="9"/>
     </row>
     <row r="135" spans="1:2">
       <c r="A135" s="8" t="s">
-        <v>92</v>
+        <v>152</v>
       </c>
       <c r="B135" s="9" t="s">
-        <v>93</v>
+        <v>153</v>
       </c>
     </row>
     <row r="136" spans="1:2">
       <c r="A136" s="8"/>
       <c r="B136" s="9" t="s">
-        <v>94</v>
+        <v>154</v>
       </c>
     </row>
     <row r="137" spans="1:2">
       <c r="A137" s="8"/>
       <c r="B137" s="9" t="s">
-        <v>64</v>
+        <v>124</v>
       </c>
     </row>
     <row r="138" spans="1:2">
       <c r="A138" s="8"/>
       <c r="B138" s="9" t="s">
-        <v>106</v>
+        <v>58</v>
       </c>
     </row>
     <row r="139" spans="1:2">
       <c r="A139" s="8" t="s">
-        <v>95</v>
+        <v>155</v>
       </c>
       <c r="B139" s="9" t="s">
-        <v>65</v>
+        <v>125</v>
       </c>
     </row>
     <row r="140" spans="1:2">
       <c r="A140" s="8"/>
       <c r="B140" s="9" t="s">
-        <v>57</v>
+        <v>117</v>
       </c>
     </row>
     <row r="141" spans="1:2">
       <c r="A141" s="8" t="s">
-        <v>58</v>
+        <v>118</v>
       </c>
       <c r="B141" s="9"/>
     </row>
     <row r="142" spans="1:2">
       <c r="A142" s="8" t="s">
-        <v>59</v>
+        <v>119</v>
       </c>
       <c r="B142" s="9"/>
     </row>
     <row r="143" spans="1:2">
       <c r="A143" s="8"/>
       <c r="B143" s="9" t="s">
-        <v>60</v>
+        <v>120</v>
       </c>
     </row>
     <row r="144" spans="1:2">
       <c r="A144" s="8"/>
       <c r="B144" s="9" t="s">
-        <v>61</v>
+        <v>121</v>
       </c>
     </row>
     <row r="145" spans="1:2">
       <c r="A145" s="8"/>
       <c r="B145" s="9" t="s">
-        <v>106</v>
+        <v>58</v>
       </c>
     </row>
     <row r="146" spans="1:2">
       <c r="A146" s="8"/>
       <c r="B146" s="9" t="s">
-        <v>62</v>
+        <v>122</v>
       </c>
     </row>
     <row r="147" spans="1:2">
       <c r="A147" s="8"/>
       <c r="B147" s="9" t="s">
-        <v>63</v>
+        <v>123</v>
       </c>
     </row>
     <row r="148" spans="1:2">
       <c r="A148" s="8" t="s">
-        <v>69</v>
+        <v>129</v>
       </c>
       <c r="B148" s="9" t="s">
-        <v>66</v>
+        <v>126</v>
       </c>
     </row>
     <row r="149" spans="1:2">
       <c r="A149" s="8"/>
       <c r="B149" s="9" t="s">
-        <v>67</v>
+        <v>127</v>
       </c>
     </row>
     <row r="150" spans="1:2">
       <c r="A150" s="8"/>
       <c r="B150" s="9" t="s">
-        <v>106</v>
+        <v>58</v>
       </c>
     </row>
     <row r="151" spans="1:2">
       <c r="A151" s="8"/>
       <c r="B151" s="9" t="s">
-        <v>70</v>
+        <v>130</v>
       </c>
     </row>
     <row r="152" spans="1:2">
       <c r="A152" s="8"/>
       <c r="B152" s="9" t="s">
-        <v>68</v>
+        <v>128</v>
       </c>
     </row>
     <row r="153" spans="1:2">
       <c r="A153" s="6" t="s">
-        <v>71</v>
+        <v>131</v>
       </c>
       <c r="B153" s="7" t="s">
-        <v>72</v>
+        <v>132</v>
       </c>
     </row>
     <row r="154" spans="1:2">
       <c r="A154" s="8"/>
       <c r="B154" s="9" t="s">
-        <v>76</v>
+        <v>136</v>
       </c>
     </row>
     <row r="155" spans="1:2">
       <c r="A155" s="8"/>
       <c r="B155" s="9" t="s">
-        <v>73</v>
+        <v>133</v>
       </c>
     </row>
     <row r="156" spans="1:2">
       <c r="A156" s="8" t="s">
-        <v>74</v>
+        <v>134</v>
       </c>
       <c r="B156" s="9" t="s">
-        <v>75</v>
+        <v>135</v>
       </c>
     </row>
     <row r="157" spans="1:2">
       <c r="A157" s="8"/>
       <c r="B157" s="9" t="s">
-        <v>55</v>
+        <v>115</v>
       </c>
     </row>
     <row r="158" spans="1:2">
       <c r="A158" s="8"/>
       <c r="B158" s="9" t="s">
-        <v>54</v>
+        <v>114</v>
       </c>
     </row>
     <row r="159" spans="1:2">
       <c r="A159" s="8"/>
       <c r="B159" s="9" t="s">
-        <v>77</v>
+        <v>137</v>
       </c>
     </row>
     <row r="160" spans="1:2">
       <c r="A160" s="8"/>
       <c r="B160" s="9" t="s">
-        <v>38</v>
+        <v>197</v>
       </c>
     </row>
     <row r="161" spans="1:2">
       <c r="A161" s="10"/>
       <c r="B161" s="11" t="s">
-        <v>39</v>
+        <v>198</v>
       </c>
     </row>
     <row r="183" spans="1:2">
       <c r="A183" s="13" t="s">
-        <v>10</v>
+        <v>169</v>
       </c>
       <c r="B183" s="7"/>
     </row>
     <row r="184" spans="1:2">
       <c r="A184" s="8" t="s">
-        <v>40</v>
+        <v>199</v>
       </c>
       <c r="B184" s="9"/>
     </row>
     <row r="185" spans="1:2">
       <c r="A185" s="8" t="s">
-        <v>41</v>
+        <v>200</v>
       </c>
       <c r="B185" s="9"/>
     </row>
     <row r="186" spans="1:2">
       <c r="A186" s="14" t="s">
-        <v>11</v>
+        <v>170</v>
       </c>
       <c r="B186" s="9"/>
     </row>
     <row r="187" spans="1:2">
       <c r="A187" s="8" t="s">
-        <v>47</v>
+        <v>206</v>
       </c>
       <c r="B187" s="9" t="s">
-        <v>46</v>
+        <v>205</v>
       </c>
     </row>
     <row r="188" spans="1:2">
       <c r="A188" s="8" t="s">
-        <v>50</v>
+        <v>110</v>
       </c>
       <c r="B188" s="9" t="s">
-        <v>48</v>
+        <v>108</v>
       </c>
     </row>
     <row r="189" spans="1:2">
       <c r="A189" s="8" t="s">
-        <v>51</v>
+        <v>111</v>
       </c>
       <c r="B189" s="9" t="s">
-        <v>49</v>
+        <v>109</v>
       </c>
     </row>
     <row r="190" spans="1:2">
       <c r="A190" s="8" t="s">
-        <v>52</v>
+        <v>112</v>
       </c>
       <c r="B190" s="9" t="s">
-        <v>53</v>
+        <v>113</v>
       </c>
     </row>
     <row r="191" spans="1:2">
       <c r="A191" s="8"/>
       <c r="B191" s="9" t="s">
-        <v>16</v>
+        <v>175</v>
       </c>
     </row>
     <row r="192" spans="1:2">
       <c r="A192" s="8"/>
       <c r="B192" s="9" t="s">
-        <v>14</v>
+        <v>173</v>
       </c>
     </row>
     <row r="193" spans="1:2">
       <c r="A193" s="8"/>
       <c r="B193" s="9" t="s">
-        <v>106</v>
+        <v>58</v>
       </c>
     </row>
     <row r="194" spans="1:2">
       <c r="A194" s="8"/>
       <c r="B194" s="9" t="s">
-        <v>56</v>
+        <v>116</v>
       </c>
     </row>
     <row r="195" spans="1:2">
       <c r="A195" s="8"/>
       <c r="B195" s="9" t="s">
-        <v>17</v>
+        <v>176</v>
       </c>
     </row>
     <row r="196" spans="1:2">
       <c r="A196" s="8"/>
       <c r="B196" s="9" t="s">
-        <v>15</v>
+        <v>174</v>
       </c>
     </row>
     <row r="197" spans="1:2">
       <c r="A197" s="8"/>
       <c r="B197" s="9" t="s">
-        <v>35</v>
+        <v>194</v>
       </c>
     </row>
     <row r="198" spans="1:2">
       <c r="A198" s="8"/>
       <c r="B198" s="9" t="s">
-        <v>106</v>
+        <v>58</v>
       </c>
     </row>
     <row r="199" spans="1:2">
       <c r="A199" s="8"/>
       <c r="B199" s="9" t="s">
-        <v>18</v>
+        <v>177</v>
       </c>
     </row>
     <row r="200" spans="1:2">
@@ -2444,67 +2502,67 @@
     <row r="201" spans="1:2">
       <c r="A201" s="8"/>
       <c r="B201" s="9" t="s">
-        <v>26</v>
+        <v>185</v>
       </c>
     </row>
     <row r="202" spans="1:2">
       <c r="A202" s="8"/>
       <c r="B202" s="9" t="s">
-        <v>27</v>
+        <v>186</v>
       </c>
     </row>
     <row r="203" spans="1:2">
       <c r="A203" s="8"/>
       <c r="B203" s="9" t="s">
-        <v>28</v>
+        <v>187</v>
       </c>
     </row>
     <row r="204" spans="1:2">
       <c r="A204" s="8"/>
       <c r="B204" s="9" t="s">
-        <v>29</v>
+        <v>188</v>
       </c>
     </row>
     <row r="205" spans="1:2">
       <c r="A205" s="14" t="s">
-        <v>12</v>
+        <v>171</v>
       </c>
       <c r="B205" s="9" t="s">
-        <v>21</v>
+        <v>180</v>
       </c>
     </row>
     <row r="206" spans="1:2">
       <c r="A206" s="8" t="s">
-        <v>19</v>
+        <v>178</v>
       </c>
       <c r="B206" s="9" t="s">
-        <v>22</v>
+        <v>181</v>
       </c>
     </row>
     <row r="207" spans="1:2">
       <c r="A207" s="8" t="s">
-        <v>20</v>
+        <v>179</v>
       </c>
       <c r="B207" s="9" t="s">
-        <v>23</v>
+        <v>182</v>
       </c>
     </row>
     <row r="208" spans="1:2">
       <c r="A208" s="8"/>
       <c r="B208" s="9" t="s">
-        <v>24</v>
+        <v>183</v>
       </c>
     </row>
     <row r="209" spans="1:2">
       <c r="A209" s="8"/>
       <c r="B209" s="9" t="s">
-        <v>106</v>
+        <v>58</v>
       </c>
     </row>
     <row r="210" spans="1:2">
       <c r="A210" s="8"/>
       <c r="B210" s="9" t="s">
-        <v>25</v>
+        <v>184</v>
       </c>
     </row>
     <row r="211" spans="1:2">
@@ -2514,31 +2572,31 @@
     <row r="212" spans="1:2">
       <c r="A212" s="8"/>
       <c r="B212" s="9" t="s">
-        <v>30</v>
+        <v>189</v>
       </c>
     </row>
     <row r="213" spans="1:2">
       <c r="A213" s="8"/>
       <c r="B213" s="9" t="s">
-        <v>31</v>
+        <v>190</v>
       </c>
     </row>
     <row r="214" spans="1:2">
       <c r="A214" s="8"/>
       <c r="B214" s="9" t="s">
-        <v>32</v>
+        <v>191</v>
       </c>
     </row>
     <row r="215" spans="1:2">
       <c r="A215" s="8"/>
       <c r="B215" s="9" t="s">
-        <v>33</v>
+        <v>192</v>
       </c>
     </row>
     <row r="216" spans="1:2">
       <c r="A216" s="10"/>
       <c r="B216" s="11" t="s">
-        <v>34</v>
+        <v>193</v>
       </c>
     </row>
   </sheetData>
@@ -2546,11 +2604,11 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup scale="81" fitToHeight="4" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <rowBreaks count="1" manualBreakCount="1">
-    <brk id="106" max="16383" man="1"/>
+    <brk id="110" max="16383" man="1"/>
   </rowBreaks>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
-      <mx:PLV Mode="0" OnePage="0" WScale="100"/>
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>
 </worksheet>

</xml_diff>